<commit_message>
Created PDF of interlocking table
</commit_message>
<xml_diff>
--- a/configurations/swtbahn-ultraloop/interlocking_table_old.xlsx
+++ b/configurations/swtbahn-ultraloop/interlocking_table_old.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugeneyip/Documents/SWTbahn/Software/swtbahn-cli/configurations/swtbahn-ultraloop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E33376F-83BB-5042-81BE-9F89A87F2AF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6FEFB5-A312-104F-A5DA-FFB5B35508CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="-16120" windowWidth="23340" windowHeight="15000" xr2:uid="{F448522D-F72F-1E4C-8C66-E38C0A38E452}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F448522D-F72F-1E4C-8C66-E38C0A38E452}"/>
   </bookViews>
   <sheets>
     <sheet name="SWTbahn Ultraloop" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -184,11 +184,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -200,6 +209,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,7 +726,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.3"/>
@@ -966,25 +979,26 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>